<commit_message>
added recovered date for GP05MOAS-GL523
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP05MOAS-GL523_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP05MOAS-GL523_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="10620" windowWidth="29865" windowHeight="10605" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="5540" yWindow="2720" windowWidth="25600" windowHeight="16060" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -35,7 +30,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$94</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$379</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -561,7 +556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,7 +591,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -807,24 +802,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="35.42578125" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="11" width="11.1640625" customWidth="1"/>
+    <col min="12" max="12" width="35.5" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28">
       <c r="A1" s="26" t="s">
         <v>29</v>
       </c>
@@ -862,7 +857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="15">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -881,7 +876,9 @@
       <c r="F2" s="7">
         <v>0.19444444444444445</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="22">
+        <v>42610</v>
+      </c>
       <c r="H2" s="23" t="s">
         <v>27</v>
       </c>
@@ -919,24 +916,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -962,7 +959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="1" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>23</v>
       </c>
@@ -991,7 +988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1020,7 +1017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="1" customFormat="1">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1078,7 +1075,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="1" customFormat="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="18"/>
@@ -1094,7 +1091,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="1" customFormat="1">
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
@@ -1124,7 +1121,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="1" customFormat="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="18"/>
@@ -1140,7 +1137,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="1" customFormat="1">
       <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
@@ -1170,7 +1167,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="1" customFormat="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="18"/>
@@ -1186,7 +1183,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
     </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="1" customFormat="1">
       <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
@@ -1216,7 +1213,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
     </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="1" customFormat="1">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="11"/>

</xml_diff>